<commit_message>
Updated with more Movies
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -31732,7 +31732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G69"/>
+  <dimension ref="A2:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -34063,6 +34063,356 @@
       <c r="G69" t="inlineStr">
         <is>
           <t>Aaron Sorkin,Walter Isaacson</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Moon</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2009-07-10</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Sam Rockwell,Kevin Spacey,Dominique McElligott</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Duncan Jones</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Duncan Jones,Nathan Parker</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Night at the Museum</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2006-12-22</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Ben Stiller,Carla Gugino,Ricky Gervais</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Shawn Levy</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Robert Ben Garant,Thomas Lennon,Milan Trenc</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Night at the Museum: Battle of the Smithsonian</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>6</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2009-05-22</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Ben Stiller,Owen Wilson,Amy Adams</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Shawn Levy</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Robert Ben Garant,Thomas Lennon</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Lego: The Adventures of Clutch Powers</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Not Rated</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2010-06-10</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Ryan McPartlin,Yvonne Strahovski,Paul Michael Glaser</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Howard E. Baker</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Tom Rogers,Joshua Wexler,Ole Kirk Christiansen</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>12 Angry Men</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>9</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>1957-04-10</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Henry Fonda,Lee J. Cobb,Martin Balsam</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Sidney Lumet</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Reginald Rose</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Purple Rain</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>1984-07-27</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Prince,Apollonia Kotero,Morris Day</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Albert Magnoli</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Albert Magnoli,William Blinn</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Hereditary</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2018-06-08</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Toni Collette,Milly Shapiro,Gabriel Byrne</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Ari Aster</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Ari Aster</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Sin City</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>8</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2005-04-01</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Mickey Rourke,Clive Owen,Bruce Willis</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Frank Miller,Quentin Tarantino,Robert Rodriguez</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Frank Miller,Robert Rodriguez</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>The Cabin in the Woods</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>7</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2012-04-13</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Kristen Connolly,Chris Hemsworth,Anna Hutchison</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Drew Goddard</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Joss Whedon,Drew Goddard</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Happy Gilmore</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>7</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>1996-02-16</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Adam Sandler,Christopher McDonald,Julie Bowen</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Dennis Dugan</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Tim Herlihy,Adam Sandler</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added batch files to allow the user to run the requirement install and script more easily
</commit_message>
<xml_diff>
--- a/Movies.xlsx
+++ b/Movies.xlsx
@@ -31732,7 +31732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G767"/>
+  <dimension ref="A2:H767"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -37413,11 +37413,16 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
+          <t>Comedy</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
           <t>Kar Lok Chin,Louisa So,Ting-Yan Wu</t>
         </is>
       </c>
-      <c r="F164" t="inlineStr"/>
       <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -37915,9 +37920,37 @@
           <t>The Adventures of Tintin</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B179" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2011-12-21</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Animation,Action,Adventure</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Jamie Bell,Andy Serkis,Daniel Craig</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>Steven Spielberg</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Hergé,Steven Moffat,Edgar Wright</t>
         </is>
       </c>
     </row>
@@ -40061,12 +40094,40 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>The Italian Job (1969)</t>
-        </is>
-      </c>
-      <c r="B242" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>The Italian Job</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>1969-09-03</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Action,Comedy,Crime</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>Michael Caine,Noël Coward,Benny Hill</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>Peter Collinson</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>Troy Kennedy-Martin</t>
         </is>
       </c>
     </row>
@@ -40281,9 +40342,37 @@
           <t>The Princess Bride</t>
         </is>
       </c>
-      <c r="B249" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B249" t="n">
+        <v>8</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>1987-10-09</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Adventure,Comedy,Family</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>Cary Elwes,Mandy Patinkin,Robin Wright</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>Rob Reiner</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>William Goldman</t>
         </is>
       </c>
     </row>
@@ -40508,9 +40597,14 @@
           <t>1974-01-26</t>
         </is>
       </c>
-      <c r="E256" t="inlineStr"/>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>Fantasy,Horror,Mystery</t>
+        </is>
+      </c>
       <c r="F256" t="inlineStr"/>
       <c r="G256" t="inlineStr"/>
+      <c r="H256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -41225,15 +41319,20 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
+          <t>Comedy</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
           <t>Sean Moore</t>
         </is>
       </c>
-      <c r="F277" t="inlineStr">
+      <c r="G277" t="inlineStr">
         <is>
           <t>Sean Moore</t>
         </is>
       </c>
-      <c r="G277" t="inlineStr">
+      <c r="H277" t="inlineStr">
         <is>
           <t>Sean Moore</t>
         </is>
@@ -41532,15 +41631,20 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
+          <t>Comedy,Talk-Show</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
           <t>Torey Gerace</t>
         </is>
       </c>
-      <c r="F286" t="inlineStr">
+      <c r="G286" t="inlineStr">
         <is>
           <t>Torey Gerace</t>
         </is>
       </c>
-      <c r="G286" t="inlineStr">
+      <c r="H286" t="inlineStr">
         <is>
           <t>Torey Gerace</t>
         </is>
@@ -41864,12 +41968,40 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Lord of the Rings: The Return of the King</t>
-        </is>
-      </c>
-      <c r="B296" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>The Lord of the Rings: The Return of the King</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>9</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>2003-12-17</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Action,Adventure,Drama</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>Elijah Wood,Viggo Mortensen,Ian McKellen</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>Peter Jackson</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>J.R.R. Tolkien,Fran Walsh,Philippa Boyens</t>
         </is>
       </c>
     </row>
@@ -42203,12 +42335,40 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Beetlejuice</t>
-        </is>
-      </c>
-      <c r="B307" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>Beetle Juice</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>1988-03-30</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Comedy,Fantasy</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>Alec Baldwin,Geena Davis,Michael Keaton</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>Tim Burton</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>Michael McDowell,Larry Wilson,Warren Skaaren</t>
         </is>
       </c>
     </row>
@@ -42470,15 +42630,20 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
+          <t>Action,Crime,Mystery</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
           <t>Vin Diesel,Jordana Brewster,Tyrese Gibson</t>
         </is>
       </c>
-      <c r="F315" t="inlineStr">
+      <c r="G315" t="inlineStr">
         <is>
           <t>Louis Leterrier</t>
         </is>
       </c>
-      <c r="G315" t="inlineStr">
+      <c r="H315" t="inlineStr">
         <is>
           <t>Justin Lin,Dan Mazeau,Gary Scott Thompson</t>
         </is>
@@ -42697,11 +42862,16 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
+          <t>Short,Action</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
           <t>Robert Patrick,Don LaFontaine,Edward Furlong</t>
         </is>
       </c>
-      <c r="F322" t="inlineStr"/>
       <c r="G322" t="inlineStr"/>
+      <c r="H322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -42716,15 +42886,20 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
+          <t>Talk-Show</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
           <t>Tamara Chambers,Jake Jarvi</t>
         </is>
       </c>
-      <c r="F323" t="inlineStr">
+      <c r="G323" t="inlineStr">
         <is>
           <t>Tamara Chambers</t>
         </is>
       </c>
-      <c r="G323" t="inlineStr">
+      <c r="H323" t="inlineStr">
         <is>
           <t>Tamara Chambers,Jake Jarvi</t>
         </is>
@@ -43016,9 +43191,37 @@
           <t>Full Metal Jacket</t>
         </is>
       </c>
-      <c r="B332" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B332" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>1987-07-10</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>Drama,War</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>Matthew Modine,R. Lee Ermey,Vincent D&amp;apos;Onofrio</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>Stanley Kubrick</t>
+        </is>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>Stanley Kubrick,Michael Herr,Gustav Hasford</t>
         </is>
       </c>
     </row>
@@ -43610,15 +43813,20 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
+          <t>Comedy</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
           <t>Hunter</t>
         </is>
       </c>
-      <c r="F350" t="inlineStr">
+      <c r="G350" t="inlineStr">
         <is>
           <t>Hunter</t>
         </is>
       </c>
-      <c r="G350" t="inlineStr">
+      <c r="H350" t="inlineStr">
         <is>
           <t>Hunter</t>
         </is>
@@ -43777,9 +43985,37 @@
           <t>The Dark Crystal</t>
         </is>
       </c>
-      <c r="B356" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B356" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>1982-12-17</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>Adventure,Family,Fantasy</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>Jim Henson,Kathryn Mullen,Frank Oz</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>Jim Henson,Frank Oz</t>
+        </is>
+      </c>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>David Odell,Jim Henson</t>
         </is>
       </c>
     </row>
@@ -44011,9 +44247,37 @@
           <t>The Cat in the Hat</t>
         </is>
       </c>
-      <c r="B364" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B364" t="n">
+        <v>4</v>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>2003-11-21</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>Adventure,Comedy,Family</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>Mike Myers,Spencer Breslin,Dakota Fanning</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>Bo Welch</t>
+        </is>
+      </c>
+      <c r="H364" t="inlineStr">
+        <is>
+          <t>Dr. Seuss,Alec Berg,David Mandel</t>
         </is>
       </c>
     </row>
@@ -44055,12 +44319,40 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>Silence of the Lambs</t>
-        </is>
-      </c>
-      <c r="B366" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>The Silence of the Lambs</t>
+        </is>
+      </c>
+      <c r="B366" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>1991-02-14</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>Crime,Drama,Thriller</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>Jodie Foster,Anthony Hopkins,Lawrence A. Bonney</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>Jonathan Demme</t>
+        </is>
+      </c>
+      <c r="H366" t="inlineStr">
+        <is>
+          <t>Thomas Harris,Ted Tally</t>
         </is>
       </c>
     </row>
@@ -45089,12 +45381,40 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>Scary Movie V</t>
-        </is>
-      </c>
-      <c r="B397" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>Scary Movie 5</t>
+        </is>
+      </c>
+      <c r="B397" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>2013-04-12</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>Comedy,Horror</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>Simon Rex,Ashley Tisdale,Charlie Sheen</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Malcolm D. Lee,David Zucker</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>David Zucker,Pat Proft,Shawn Wayans</t>
         </is>
       </c>
     </row>
@@ -45631,15 +45951,20 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
+          <t>Action,Adventure,Comedy</t>
+        </is>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
           <t>Ormsby,Eric Rodriguez</t>
         </is>
       </c>
-      <c r="F413" t="inlineStr">
+      <c r="G413" t="inlineStr">
         <is>
           <t>Eric Rodriguez</t>
         </is>
       </c>
-      <c r="G413" t="inlineStr">
+      <c r="H413" t="inlineStr">
         <is>
           <t>Eric Rodriguez</t>
         </is>
@@ -46133,12 +46458,40 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>It: Chapter 1</t>
-        </is>
-      </c>
-      <c r="B428" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>It</t>
+        </is>
+      </c>
+      <c r="B428" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>2017-09-08</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>Horror</t>
+        </is>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>Bill Skarsgård,Jaeden Martell,Finn Wolfhard</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>Andy Muschietti</t>
+        </is>
+      </c>
+      <c r="H428" t="inlineStr">
+        <is>
+          <t>Chase Palmer,Cary Joji Fukunaga,Gary Dauberman</t>
         </is>
       </c>
     </row>
@@ -46183,9 +46536,37 @@
           <t>Clash of the Titans</t>
         </is>
       </c>
-      <c r="B430" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B430" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>1981-06-12</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>Action,Adventure,Family</t>
+        </is>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t>Laurence Olivier,Harry Hamlin,Claire Bloom</t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t>Desmond Davis</t>
+        </is>
+      </c>
+      <c r="H430" t="inlineStr">
+        <is>
+          <t>Beverley Cross</t>
         </is>
       </c>
     </row>
@@ -46370,9 +46751,37 @@
           <t>Johnny English</t>
         </is>
       </c>
-      <c r="B436" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B436" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>2003-07-18</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>Action,Adventure,Comedy</t>
+        </is>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>Rowan Atkinson,John Malkovich,Natalie Imbruglia</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>Peter Howitt</t>
+        </is>
+      </c>
+      <c r="H436" t="inlineStr">
+        <is>
+          <t>Neal Purvis,Robert Wade,Will Davies</t>
         </is>
       </c>
     </row>
@@ -46417,9 +46826,37 @@
           <t>The Spy Next Door</t>
         </is>
       </c>
-      <c r="B438" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B438" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>2010-01-15</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>Action,Comedy,Family</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>Jackie Chan,Amber Valletta,Billy Ray Cyrus</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>Brian Levant</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>Jonathan Bernstein,James Greer,Gregory Poirier</t>
         </is>
       </c>
     </row>
@@ -47298,9 +47735,37 @@
           <t>A.I. Artificial Intelligence</t>
         </is>
       </c>
-      <c r="B466" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B466" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>2001-06-29</t>
+        </is>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>Drama,Sci-Fi</t>
+        </is>
+      </c>
+      <c r="F466" t="inlineStr">
+        <is>
+          <t>Haley Joel Osment,Jude Law,Frances O&amp;apos;Connor</t>
+        </is>
+      </c>
+      <c r="G466" t="inlineStr">
+        <is>
+          <t>Steven Spielberg</t>
+        </is>
+      </c>
+      <c r="H466" t="inlineStr">
+        <is>
+          <t>Brian Aldiss,Ian Watson,Steven Spielberg</t>
         </is>
       </c>
     </row>
@@ -47940,9 +48405,37 @@
           <t>Home Alone</t>
         </is>
       </c>
-      <c r="B485" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B485" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>1990-11-16</t>
+        </is>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>Comedy,Family</t>
+        </is>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>Macaulay Culkin,Joe Pesci,Daniel Stern</t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t>Chris Columbus</t>
+        </is>
+      </c>
+      <c r="H485" t="inlineStr">
+        <is>
+          <t>John Hughes</t>
         </is>
       </c>
     </row>
@@ -49279,15 +49772,20 @@
       </c>
       <c r="E524" t="inlineStr">
         <is>
+          <t>Adventure</t>
+        </is>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
           <t>Hurricane360,MissLink8908</t>
         </is>
       </c>
-      <c r="F524" t="inlineStr">
+      <c r="G524" t="inlineStr">
         <is>
           <t>Fredrik Nilsson</t>
         </is>
       </c>
-      <c r="G524" t="inlineStr">
+      <c r="H524" t="inlineStr">
         <is>
           <t>Fredrik Nilsson,Tony Salazar</t>
         </is>
@@ -49306,15 +49804,20 @@
       </c>
       <c r="E525" t="inlineStr">
         <is>
+          <t>Comedy,Talk-Show</t>
+        </is>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
           <t>Jack Vogt</t>
         </is>
       </c>
-      <c r="F525" t="inlineStr">
+      <c r="G525" t="inlineStr">
         <is>
           <t>Jack Vogt</t>
         </is>
       </c>
-      <c r="G525" t="inlineStr">
+      <c r="H525" t="inlineStr">
         <is>
           <t>Jack Vogt</t>
         </is>
@@ -50258,12 +50761,40 @@
     <row r="553">
       <c r="A553" t="inlineStr">
         <is>
-          <t>Seven Samurai</t>
-        </is>
-      </c>
-      <c r="B553" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>Shichinin no samurai</t>
+        </is>
+      </c>
+      <c r="B553" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>Not Rated</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>1956-11-19</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
+        <is>
+          <t>Action,Drama</t>
+        </is>
+      </c>
+      <c r="F553" t="inlineStr">
+        <is>
+          <t>Toshirô Mifune,Takashi Shimura,Keiko Tsushima</t>
+        </is>
+      </c>
+      <c r="G553" t="inlineStr">
+        <is>
+          <t>Akira Kurosawa</t>
+        </is>
+      </c>
+      <c r="H553" t="inlineStr">
+        <is>
+          <t>Akira Kurosawa,Shinobu Hashimoto,Hideo Oguni</t>
         </is>
       </c>
     </row>
@@ -50343,9 +50874,37 @@
           <t>The Lost Boys</t>
         </is>
       </c>
-      <c r="B556" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B556" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>1987-07-31</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>Comedy,Horror</t>
+        </is>
+      </c>
+      <c r="F556" t="inlineStr">
+        <is>
+          <t>Jason Patric,Corey Haim,Dianne Wiest</t>
+        </is>
+      </c>
+      <c r="G556" t="inlineStr">
+        <is>
+          <t>Joel Schumacher</t>
+        </is>
+      </c>
+      <c r="H556" t="inlineStr">
+        <is>
+          <t>Jan Fischer,James Jeremias,Jeffrey Boam</t>
         </is>
       </c>
     </row>
@@ -50472,15 +51031,20 @@
       </c>
       <c r="E560" t="inlineStr">
         <is>
+          <t>Talk-Show</t>
+        </is>
+      </c>
+      <c r="F560" t="inlineStr">
+        <is>
           <t>Jeremy Jahns</t>
         </is>
       </c>
-      <c r="F560" t="inlineStr">
+      <c r="G560" t="inlineStr">
         <is>
           <t>Jeremy Jahns</t>
         </is>
       </c>
-      <c r="G560" t="inlineStr">
+      <c r="H560" t="inlineStr">
         <is>
           <t>Jeremy Jahns</t>
         </is>
@@ -50569,15 +51133,20 @@
       </c>
       <c r="E563" t="inlineStr">
         <is>
+          <t>Comedy,Horror</t>
+        </is>
+      </c>
+      <c r="F563" t="inlineStr">
+        <is>
           <t>Rob Boor,Sean Moore</t>
         </is>
       </c>
-      <c r="F563" t="inlineStr">
+      <c r="G563" t="inlineStr">
         <is>
           <t>Rob Boor</t>
         </is>
       </c>
-      <c r="G563" t="inlineStr">
+      <c r="H563" t="inlineStr">
         <is>
           <t>Rob Boor</t>
         </is>
@@ -50869,9 +51438,37 @@
           <t>The Cable Guy</t>
         </is>
       </c>
-      <c r="B572" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B572" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>1996-06-14</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr">
+        <is>
+          <t>Comedy,Drama,Thriller</t>
+        </is>
+      </c>
+      <c r="F572" t="inlineStr">
+        <is>
+          <t>Jim Carrey,Matthew Broderick,Leslie Mann</t>
+        </is>
+      </c>
+      <c r="G572" t="inlineStr">
+        <is>
+          <t>Ben Stiller</t>
+        </is>
+      </c>
+      <c r="H572" t="inlineStr">
+        <is>
+          <t>Lou Holtz Jr.</t>
         </is>
       </c>
     </row>
@@ -51168,15 +51765,20 @@
       </c>
       <c r="E581" t="inlineStr">
         <is>
+          <t>Talk-Show</t>
+        </is>
+      </c>
+      <c r="F581" t="inlineStr">
+        <is>
           <t>Chris Dandridge</t>
         </is>
       </c>
-      <c r="F581" t="inlineStr">
+      <c r="G581" t="inlineStr">
         <is>
           <t>Chris Dandridge</t>
         </is>
       </c>
-      <c r="G581" t="inlineStr">
+      <c r="H581" t="inlineStr">
         <is>
           <t>Chris Dandridge</t>
         </is>
@@ -51503,9 +52105,37 @@
           <t>Halloween H20: 20 Years Later</t>
         </is>
       </c>
-      <c r="B591" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B591" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>1998-08-05</t>
+        </is>
+      </c>
+      <c r="E591" t="inlineStr">
+        <is>
+          <t>Horror,Thriller</t>
+        </is>
+      </c>
+      <c r="F591" t="inlineStr">
+        <is>
+          <t>Jamie Lee Curtis,Josh Hartnett,Adam Arkin</t>
+        </is>
+      </c>
+      <c r="G591" t="inlineStr">
+        <is>
+          <t>Steve Miner</t>
+        </is>
+      </c>
+      <c r="H591" t="inlineStr">
+        <is>
+          <t>Debra Hill,John Carpenter,Robert Zappia</t>
         </is>
       </c>
     </row>
@@ -51690,9 +52320,37 @@
           <t>Black Widow</t>
         </is>
       </c>
-      <c r="B597" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B597" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>2021-07-09</t>
+        </is>
+      </c>
+      <c r="E597" t="inlineStr">
+        <is>
+          <t>Action,Adventure,Sci-Fi</t>
+        </is>
+      </c>
+      <c r="F597" t="inlineStr">
+        <is>
+          <t>Scarlett Johansson,Florence Pugh,David Harbour</t>
+        </is>
+      </c>
+      <c r="G597" t="inlineStr">
+        <is>
+          <t>Cate Shortland</t>
+        </is>
+      </c>
+      <c r="H597" t="inlineStr">
+        <is>
+          <t>Eric Pearson,Jac Schaeffer,Ned Benson</t>
         </is>
       </c>
     </row>
@@ -52408,9 +53066,14 @@
           <t>2014-03-17</t>
         </is>
       </c>
-      <c r="E620" t="inlineStr"/>
+      <c r="E620" t="inlineStr">
+        <is>
+          <t>Documentary,Animation,Action</t>
+        </is>
+      </c>
       <c r="F620" t="inlineStr"/>
       <c r="G620" t="inlineStr"/>
+      <c r="H620" t="inlineStr"/>
     </row>
     <row r="621">
       <c r="A621" t="inlineStr">
@@ -52418,9 +53081,37 @@
           <t>The Haunting in Connecticut</t>
         </is>
       </c>
-      <c r="B621" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B621" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>2009-03-27</t>
+        </is>
+      </c>
+      <c r="E621" t="inlineStr">
+        <is>
+          <t>Drama,Horror,Mystery</t>
+        </is>
+      </c>
+      <c r="F621" t="inlineStr">
+        <is>
+          <t>Virginia Madsen,Martin Donovan,Elias Koteas</t>
+        </is>
+      </c>
+      <c r="G621" t="inlineStr">
+        <is>
+          <t>Peter Cornwell</t>
+        </is>
+      </c>
+      <c r="H621" t="inlineStr">
+        <is>
+          <t>Adam Simon,Tim Metcalfe</t>
         </is>
       </c>
     </row>
@@ -52612,11 +53303,16 @@
       </c>
       <c r="E627" t="inlineStr">
         <is>
+          <t>Documentary</t>
+        </is>
+      </c>
+      <c r="F627" t="inlineStr">
+        <is>
           <t>Larry Underwood</t>
         </is>
       </c>
-      <c r="F627" t="inlineStr"/>
       <c r="G627" t="inlineStr"/>
+      <c r="H627" t="inlineStr"/>
     </row>
     <row r="628">
       <c r="A628" t="inlineStr">
@@ -52826,12 +53522,40 @@
     <row r="634">
       <c r="A634" t="inlineStr">
         <is>
-          <t xml:space="preserve">Piranha </t>
-        </is>
-      </c>
-      <c r="B634" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>Piranha</t>
+        </is>
+      </c>
+      <c r="B634" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>1978-08-03</t>
+        </is>
+      </c>
+      <c r="E634" t="inlineStr">
+        <is>
+          <t>Comedy,Horror,Sci-Fi</t>
+        </is>
+      </c>
+      <c r="F634" t="inlineStr">
+        <is>
+          <t>Bradford Dillman,Heather Menzies-Urich,Kevin McCarthy</t>
+        </is>
+      </c>
+      <c r="G634" t="inlineStr">
+        <is>
+          <t>Joe Dante</t>
+        </is>
+      </c>
+      <c r="H634" t="inlineStr">
+        <is>
+          <t>Richard Robinson,John Sayles</t>
         </is>
       </c>
     </row>
@@ -53378,9 +54102,37 @@
           <t>The Evil Dead</t>
         </is>
       </c>
-      <c r="B651" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B651" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>NC-17</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>1983-04-15</t>
+        </is>
+      </c>
+      <c r="E651" t="inlineStr">
+        <is>
+          <t>Horror</t>
+        </is>
+      </c>
+      <c r="F651" t="inlineStr">
+        <is>
+          <t>Bruce Campbell,Ellen Sandweiss,Richard DeManincor</t>
+        </is>
+      </c>
+      <c r="G651" t="inlineStr">
+        <is>
+          <t>Sam Raimi</t>
+        </is>
+      </c>
+      <c r="H651" t="inlineStr">
+        <is>
+          <t>Sam Raimi</t>
         </is>
       </c>
     </row>
@@ -54472,9 +55224,37 @@
           <t>Ever After</t>
         </is>
       </c>
-      <c r="B684" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B684" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>1998-07-31</t>
+        </is>
+      </c>
+      <c r="E684" t="inlineStr">
+        <is>
+          <t>Comedy,Drama,Romance</t>
+        </is>
+      </c>
+      <c r="F684" t="inlineStr">
+        <is>
+          <t>Drew Barrymore,Anjelica Huston,Dougray Scott</t>
+        </is>
+      </c>
+      <c r="G684" t="inlineStr">
+        <is>
+          <t>Andy Tennant</t>
+        </is>
+      </c>
+      <c r="H684" t="inlineStr">
+        <is>
+          <t>Susannah Grant,Andy Tennant,Rick Parks</t>
         </is>
       </c>
     </row>
@@ -54531,15 +55311,20 @@
       </c>
       <c r="E686" t="inlineStr">
         <is>
+          <t>Talk-Show</t>
+        </is>
+      </c>
+      <c r="F686" t="inlineStr">
+        <is>
           <t>Chris Dandridge</t>
         </is>
       </c>
-      <c r="F686" t="inlineStr">
+      <c r="G686" t="inlineStr">
         <is>
           <t>Chris Dandridge</t>
         </is>
       </c>
-      <c r="G686" t="inlineStr">
+      <c r="H686" t="inlineStr">
         <is>
           <t>Chris Dandridge</t>
         </is>
@@ -54621,9 +55406,37 @@
           <t>Marrowbone</t>
         </is>
       </c>
-      <c r="B689" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B689" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>2018-04-13</t>
+        </is>
+      </c>
+      <c r="E689" t="inlineStr">
+        <is>
+          <t>Adventure,Drama,Horror</t>
+        </is>
+      </c>
+      <c r="F689" t="inlineStr">
+        <is>
+          <t>George MacKay,Anya Taylor-Joy,Charlie Heaton</t>
+        </is>
+      </c>
+      <c r="G689" t="inlineStr">
+        <is>
+          <t>Sergio G. Sánchez</t>
+        </is>
+      </c>
+      <c r="H689" t="inlineStr">
+        <is>
+          <t>Sergio G. Sánchez</t>
         </is>
       </c>
     </row>
@@ -54665,12 +55478,40 @@
     <row r="691">
       <c r="A691" t="inlineStr">
         <is>
-          <t>Boondock Saints</t>
-        </is>
-      </c>
-      <c r="B691" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>The Boondock Saints</t>
+        </is>
+      </c>
+      <c r="B691" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>2000-01-21</t>
+        </is>
+      </c>
+      <c r="E691" t="inlineStr">
+        <is>
+          <t>Action,Thriller</t>
+        </is>
+      </c>
+      <c r="F691" t="inlineStr">
+        <is>
+          <t>Willem Dafoe,Sean Patrick Flanery,Norman Reedus</t>
+        </is>
+      </c>
+      <c r="G691" t="inlineStr">
+        <is>
+          <t>Troy Duffy</t>
+        </is>
+      </c>
+      <c r="H691" t="inlineStr">
+        <is>
+          <t>Troy Duffy</t>
         </is>
       </c>
     </row>
@@ -54785,21 +55626,77 @@
           <t>Spy Kids 3: Game Over</t>
         </is>
       </c>
-      <c r="B695" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B695" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>2003-07-25</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr">
+        <is>
+          <t>Action,Adventure,Comedy</t>
+        </is>
+      </c>
+      <c r="F695" t="inlineStr">
+        <is>
+          <t>Daryl Sabara,Alexa PenaVega,Antonio Banderas</t>
+        </is>
+      </c>
+      <c r="G695" t="inlineStr">
+        <is>
+          <t>Robert Rodriguez</t>
+        </is>
+      </c>
+      <c r="H695" t="inlineStr">
+        <is>
+          <t>Robert Rodriguez</t>
         </is>
       </c>
     </row>
     <row r="696">
       <c r="A696" t="inlineStr">
         <is>
-          <t>Astroboy</t>
-        </is>
-      </c>
-      <c r="B696" t="inlineStr">
-        <is>
-          <t>data not found</t>
+          <t>Astro Boy</t>
+        </is>
+      </c>
+      <c r="B696" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>2009-10-23</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr">
+        <is>
+          <t>Animation,Action,Adventure</t>
+        </is>
+      </c>
+      <c r="F696" t="inlineStr">
+        <is>
+          <t>Freddie Highmore,Nicolas Cage,Kristen Bell</t>
+        </is>
+      </c>
+      <c r="G696" t="inlineStr">
+        <is>
+          <t>David Bowers</t>
+        </is>
+      </c>
+      <c r="H696" t="inlineStr">
+        <is>
+          <t>Osamu Tezuka,David Bowers,Timothy Harris</t>
         </is>
       </c>
     </row>
@@ -55159,9 +56056,37 @@
           <t>Paranormal Activity 3</t>
         </is>
       </c>
-      <c r="B707" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B707" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>2011-10-21</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>Horror,Mystery</t>
+        </is>
+      </c>
+      <c r="F707" t="inlineStr">
+        <is>
+          <t>Chloe Csengery,Jessica Tyler Brown,Christopher Nicholas Smith</t>
+        </is>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>Henry Joost,Ariel Schulman</t>
+        </is>
+      </c>
+      <c r="H707" t="inlineStr">
+        <is>
+          <t>Christopher Landon,Oren Peli</t>
         </is>
       </c>
     </row>
@@ -55451,9 +56376,37 @@
           <t>Halloweentown</t>
         </is>
       </c>
-      <c r="B716" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B716" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>TV-G</t>
+        </is>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>1998-10-17</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr">
+        <is>
+          <t>Adventure,Comedy,Family</t>
+        </is>
+      </c>
+      <c r="F716" t="inlineStr">
+        <is>
+          <t>Debbie Reynolds,Kimberly J. Brown,Judith Hoag</t>
+        </is>
+      </c>
+      <c r="G716" t="inlineStr">
+        <is>
+          <t>Duwayne Dunham</t>
+        </is>
+      </c>
+      <c r="H716" t="inlineStr">
+        <is>
+          <t>Paul Bernbaum,Jon Cooksey,Ali Marie Matheson</t>
         </is>
       </c>
     </row>
@@ -55750,9 +56703,37 @@
           <t>Black Panther: Wakanda Forever</t>
         </is>
       </c>
-      <c r="B726" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B726" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>2022-11-11</t>
+        </is>
+      </c>
+      <c r="E726" t="inlineStr">
+        <is>
+          <t>Action,Adventure,Drama</t>
+        </is>
+      </c>
+      <c r="F726" t="inlineStr">
+        <is>
+          <t>Letitia Wright,Lupita Nyong&amp;apos;o,Danai Gurira</t>
+        </is>
+      </c>
+      <c r="G726" t="inlineStr">
+        <is>
+          <t>Ryan Coogler</t>
+        </is>
+      </c>
+      <c r="H726" t="inlineStr">
+        <is>
+          <t>Ryan Coogler,Joe Robert Cole,Stan Lee</t>
         </is>
       </c>
     </row>
@@ -56189,15 +57170,20 @@
       </c>
       <c r="E739" t="inlineStr">
         <is>
+          <t>Short,Fantasy,Horror</t>
+        </is>
+      </c>
+      <c r="F739" t="inlineStr">
+        <is>
           <t>Patricia Castelo Branco,Sandy Guillen,Kamal Madbooly</t>
         </is>
       </c>
-      <c r="F739" t="inlineStr">
+      <c r="G739" t="inlineStr">
         <is>
           <t>Dalton Richardson</t>
         </is>
       </c>
-      <c r="G739" t="inlineStr">
+      <c r="H739" t="inlineStr">
         <is>
           <t>Dalton Richardson</t>
         </is>
@@ -56629,9 +57615,37 @@
           <t>Signs</t>
         </is>
       </c>
-      <c r="B752" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B752" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>PG-13</t>
+        </is>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>2002-08-02</t>
+        </is>
+      </c>
+      <c r="E752" t="inlineStr">
+        <is>
+          <t>Drama,Mystery,Sci-Fi</t>
+        </is>
+      </c>
+      <c r="F752" t="inlineStr">
+        <is>
+          <t>Mel Gibson,Joaquin Phoenix,Rory Culkin</t>
+        </is>
+      </c>
+      <c r="G752" t="inlineStr">
+        <is>
+          <t>M. Night Shyamalan</t>
+        </is>
+      </c>
+      <c r="H752" t="inlineStr">
+        <is>
+          <t>M. Night Shyamalan</t>
         </is>
       </c>
     </row>
@@ -57026,9 +58040,37 @@
           <t>Twins</t>
         </is>
       </c>
-      <c r="B764" t="inlineStr">
-        <is>
-          <t>data not found</t>
+      <c r="B764" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D764" t="inlineStr">
+        <is>
+          <t>1988-12-09</t>
+        </is>
+      </c>
+      <c r="E764" t="inlineStr">
+        <is>
+          <t>Comedy,Crime</t>
+        </is>
+      </c>
+      <c r="F764" t="inlineStr">
+        <is>
+          <t>Arnold Schwarzenegger,Danny DeVito,Kelly Preston</t>
+        </is>
+      </c>
+      <c r="G764" t="inlineStr">
+        <is>
+          <t>Ivan Reitman</t>
+        </is>
+      </c>
+      <c r="H764" t="inlineStr">
+        <is>
+          <t>Will Davies,William Osborne,Timothy Harris</t>
         </is>
       </c>
     </row>

</xml_diff>